<commit_message>
retrieved processed head files from old commit
</commit_message>
<xml_diff>
--- a/SCRIPT OUTPUTS/1D temp pro/SC_sensitivity_analysis.xlsx
+++ b/SCRIPT OUTPUTS/1D temp pro/SC_sensitivity_analysis.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SecondCreekGit\SCRIPT OUTPUTS\1D temp pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Ke calculations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="25">
   <si>
     <t>Sensitivity analysis</t>
   </si>
@@ -67,6 +68,39 @@
   </si>
   <si>
     <t>B/C</t>
+  </si>
+  <si>
+    <t>Xs</t>
+  </si>
+  <si>
+    <t>Ke geometric</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Kw</t>
+  </si>
+  <si>
+    <t>Xo</t>
+  </si>
+  <si>
+    <t>Ko</t>
+  </si>
+  <si>
+    <t>Ksed</t>
+  </si>
+  <si>
+    <t>Ke unsat max</t>
+  </si>
+  <si>
+    <t>Ke unsat min</t>
+  </si>
+  <si>
+    <t>Ks unsat</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -353,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="513201320"/>
-        <c:axId val="513200536"/>
+        <c:axId val="229894624"/>
+        <c:axId val="229895016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="513201320"/>
+        <c:axId val="229894624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,12 +448,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513200536"/>
+        <c:crossAx val="229895016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="513200536"/>
+        <c:axId val="229895016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,7 +510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513201320"/>
+        <c:crossAx val="229894624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -573,7 +607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -700,11 +733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="605953944"/>
-        <c:axId val="605956688"/>
+        <c:axId val="175913552"/>
+        <c:axId val="526815680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="605953944"/>
+        <c:axId val="175913552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,12 +794,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605956688"/>
+        <c:crossAx val="526815680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="605956688"/>
+        <c:axId val="526815680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605953944"/>
+        <c:crossAx val="175913552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2314,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A12:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A20" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3118,7 +3151,7 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:21" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
@@ -3155,7 +3188,7 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="2:21" ht="27" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C45" s="5" t="s">
         <v>2</v>
       </c>
@@ -3558,4 +3591,476 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1">
+        <v>0.25</v>
+      </c>
+      <c r="C1">
+        <v>0.3</v>
+      </c>
+      <c r="D1">
+        <v>0.35</v>
+      </c>
+      <c r="E1">
+        <v>0.4</v>
+      </c>
+      <c r="F1">
+        <v>0.45</v>
+      </c>
+      <c r="G1">
+        <v>0.5</v>
+      </c>
+      <c r="H1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I1">
+        <v>0.6</v>
+      </c>
+      <c r="J1">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J2">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0.51</v>
+      </c>
+      <c r="C3">
+        <v>0.51</v>
+      </c>
+      <c r="D3">
+        <v>0.51</v>
+      </c>
+      <c r="E3">
+        <v>0.51</v>
+      </c>
+      <c r="F3">
+        <v>0.51</v>
+      </c>
+      <c r="G3">
+        <v>0.51</v>
+      </c>
+      <c r="H3">
+        <v>0.51</v>
+      </c>
+      <c r="I3">
+        <v>0.51</v>
+      </c>
+      <c r="J3">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <f>POWER(B1,1-B3)*POWER(B2,B3)</f>
+        <v>0.38061577197708579</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:J7" si="0">POWER(C1,1-C3)*POWER(C2,C3)</f>
+        <v>0.41618420244849613</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.44883789625720572</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.47918760100621</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.50765691719967043</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.53455387057828008</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.56011073225609709</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.58450777049189562</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.60788821116058367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f>1-A11</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f>A11*D11+B11*C11</f>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f>POWER((A11/D11)+(B11/C11),-1)</f>
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <f>AVERAGE(E11:F11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.9</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:B21" si="1">1-A12</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E21" si="2">A12*D12+B12*C12</f>
+        <v>1.825</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F21" si="3">POWER((A12/D12)+(B12/C12),-1)</f>
+        <v>1.1764705882352944</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G21" si="4">AVERAGE(E12:F12)</f>
+        <v>1.5007352941176473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.8</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="C13">
+        <v>0.25</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333348</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>1.2416666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.7</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C14">
+        <v>0.25</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>1.4749999999999999</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>0.64516129032258052</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>1.0600806451612903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.6</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="C15">
+        <v>0.25</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>0.91315789473684217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.5</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>0.25</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>1.125</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0.78472222222222221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.4</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="C17">
+        <v>0.25</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>0.38461538461538458</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>0.66730769230769238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.3</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="C18">
+        <v>0.25</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.77499999999999991</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0.33898305084745767</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0.55699152542372876</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="C19">
+        <v>0.25</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>0.30303030303030298</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>0.45151515151515154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.1</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="C20">
+        <v>0.25</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>0.27397260273972601</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>0.34948630136986303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.25</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>